<commit_message>
ajustes dos trts físicos; mover os arquivos concluídos
</commit_message>
<xml_diff>
--- a/Data/Reports/BANCO PACTUAL S A.xlsx
+++ b/Data/Reports/BANCO PACTUAL S A.xlsx
@@ -3201,13 +3201,33 @@
       <c r="BT19" s="1" t="n"/>
     </row>
     <row r="20" ht="15.95" customHeight="1" s="18">
-      <c r="A20" s="32" t="n"/>
+      <c r="A20" s="32" t="inlineStr">
+        <is>
+          <t>00004</t>
+        </is>
+      </c>
       <c r="B20" s="32" t="n"/>
       <c r="C20" s="32" t="n"/>
-      <c r="D20" s="32" t="n"/>
-      <c r="E20" s="49" t="n"/>
-      <c r="F20" s="49" t="n"/>
-      <c r="G20" s="89" t="n"/>
+      <c r="D20" s="32" t="inlineStr">
+        <is>
+          <t>000011265962013</t>
+        </is>
+      </c>
+      <c r="E20" s="49" t="inlineStr">
+        <is>
+          <t>BANCO PACTUAL S A</t>
+        </is>
+      </c>
+      <c r="F20" s="49" t="inlineStr">
+        <is>
+          <t>ANDREA DIAS SILVA</t>
+        </is>
+      </c>
+      <c r="G20" s="89" t="inlineStr">
+        <is>
+          <t>18.751,25</t>
+        </is>
+      </c>
       <c r="H20" s="34" t="n"/>
       <c r="I20" s="32" t="n"/>
       <c r="J20" s="32" t="n"/>
@@ -3232,11 +3252,27 @@
       <c r="AC20" s="38" t="n"/>
       <c r="AD20" s="38" t="n"/>
       <c r="AE20" s="38" t="n"/>
-      <c r="AF20" s="90" t="n"/>
-      <c r="AG20" s="90" t="n"/>
-      <c r="AH20" s="32" t="n"/>
+      <c r="AF20" s="90" t="inlineStr">
+        <is>
+          <t>09970508116543</t>
+        </is>
+      </c>
+      <c r="AG20" s="90" t="inlineStr">
+        <is>
+          <t>00000008046</t>
+        </is>
+      </c>
+      <c r="AH20" s="32" t="inlineStr">
+        <is>
+          <t>24/07/2015</t>
+        </is>
+      </c>
       <c r="AI20" s="32" t="n"/>
-      <c r="AJ20" s="32" t="n"/>
+      <c r="AJ20" s="32" t="inlineStr">
+        <is>
+          <t>00000000000</t>
+        </is>
+      </c>
       <c r="AK20" s="32" t="n"/>
       <c r="AL20" s="32" t="n"/>
       <c r="AM20" s="32" t="n"/>
@@ -3274,13 +3310,33 @@
       <c r="BT20" s="1" t="n"/>
     </row>
     <row r="21" ht="15.95" customHeight="1" s="18">
-      <c r="A21" s="32" t="n"/>
+      <c r="A21" s="32" t="inlineStr">
+        <is>
+          <t>00081</t>
+        </is>
+      </c>
       <c r="B21" s="32" t="n"/>
       <c r="C21" s="32" t="n"/>
-      <c r="D21" s="32" t="n"/>
-      <c r="E21" s="49" t="n"/>
-      <c r="F21" s="49" t="n"/>
-      <c r="G21" s="89" t="n"/>
+      <c r="D21" s="32" t="inlineStr">
+        <is>
+          <t>000000483122012</t>
+        </is>
+      </c>
+      <c r="E21" s="49" t="inlineStr">
+        <is>
+          <t>BANCO PACTUAL S A</t>
+        </is>
+      </c>
+      <c r="F21" s="49" t="inlineStr">
+        <is>
+          <t>CARLOS ALBERTO SENRA SANTOS</t>
+        </is>
+      </c>
+      <c r="G21" s="89" t="inlineStr">
+        <is>
+          <t>8.934,33</t>
+        </is>
+      </c>
       <c r="H21" s="34" t="n"/>
       <c r="I21" s="32" t="n"/>
       <c r="J21" s="32" t="n"/>
@@ -3305,11 +3361,27 @@
       <c r="AC21" s="38" t="n"/>
       <c r="AD21" s="38" t="n"/>
       <c r="AE21" s="38" t="n"/>
-      <c r="AF21" s="90" t="n"/>
-      <c r="AG21" s="90" t="n"/>
-      <c r="AH21" s="32" t="n"/>
+      <c r="AF21" s="90" t="inlineStr">
+        <is>
+          <t>09970508116543</t>
+        </is>
+      </c>
+      <c r="AG21" s="90" t="inlineStr">
+        <is>
+          <t>00000005292</t>
+        </is>
+      </c>
+      <c r="AH21" s="32" t="inlineStr">
+        <is>
+          <t>24/07/2013</t>
+        </is>
+      </c>
       <c r="AI21" s="32" t="n"/>
-      <c r="AJ21" s="32" t="n"/>
+      <c r="AJ21" s="32" t="inlineStr">
+        <is>
+          <t>00000000000</t>
+        </is>
+      </c>
       <c r="AK21" s="32" t="n"/>
       <c r="AL21" s="32" t="n"/>
       <c r="AM21" s="32" t="n"/>
@@ -3347,13 +3419,33 @@
       <c r="BT21" s="1" t="n"/>
     </row>
     <row r="22" ht="15.95" customHeight="1" s="18">
-      <c r="A22" s="32" t="n"/>
+      <c r="A22" s="32" t="inlineStr">
+        <is>
+          <t>00003</t>
+        </is>
+      </c>
       <c r="B22" s="32" t="n"/>
       <c r="C22" s="32" t="n"/>
-      <c r="D22" s="32" t="n"/>
-      <c r="E22" s="49" t="n"/>
-      <c r="F22" s="49" t="n"/>
-      <c r="G22" s="89" t="n"/>
+      <c r="D22" s="32" t="inlineStr">
+        <is>
+          <t>000001571922013</t>
+        </is>
+      </c>
+      <c r="E22" s="49" t="inlineStr">
+        <is>
+          <t>BANCO PACTUAL S A</t>
+        </is>
+      </c>
+      <c r="F22" s="49" t="inlineStr">
+        <is>
+          <t>DAIANE SANTOS PUGAS</t>
+        </is>
+      </c>
+      <c r="G22" s="89" t="inlineStr">
+        <is>
+          <t>18.921,46</t>
+        </is>
+      </c>
       <c r="H22" s="34" t="n"/>
       <c r="I22" s="32" t="n"/>
       <c r="J22" s="32" t="n"/>
@@ -3378,11 +3470,27 @@
       <c r="AC22" s="38" t="n"/>
       <c r="AD22" s="38" t="n"/>
       <c r="AE22" s="38" t="n"/>
-      <c r="AF22" s="90" t="n"/>
-      <c r="AG22" s="90" t="n"/>
-      <c r="AH22" s="32" t="n"/>
+      <c r="AF22" s="90" t="inlineStr">
+        <is>
+          <t>09970508116543</t>
+        </is>
+      </c>
+      <c r="AG22" s="90" t="inlineStr">
+        <is>
+          <t>00000007317</t>
+        </is>
+      </c>
+      <c r="AH22" s="32" t="inlineStr">
+        <is>
+          <t>09/06/2015</t>
+        </is>
+      </c>
       <c r="AI22" s="32" t="n"/>
-      <c r="AJ22" s="32" t="n"/>
+      <c r="AJ22" s="32" t="inlineStr">
+        <is>
+          <t>00000000000</t>
+        </is>
+      </c>
       <c r="AK22" s="32" t="n"/>
       <c r="AL22" s="32" t="n"/>
       <c r="AM22" s="32" t="n"/>
@@ -3420,13 +3528,33 @@
       <c r="BT22" s="1" t="n"/>
     </row>
     <row r="23" ht="15.95" customHeight="1" s="18">
-      <c r="A23" s="32" t="n"/>
+      <c r="A23" s="32" t="inlineStr">
+        <is>
+          <t>00029</t>
+        </is>
+      </c>
       <c r="B23" s="32" t="n"/>
       <c r="C23" s="32" t="n"/>
-      <c r="D23" s="32" t="n"/>
-      <c r="E23" s="49" t="n"/>
-      <c r="F23" s="49" t="n"/>
-      <c r="G23" s="89" t="n"/>
+      <c r="D23" s="32" t="inlineStr">
+        <is>
+          <t>000200302901005</t>
+        </is>
+      </c>
+      <c r="E23" s="49" t="inlineStr">
+        <is>
+          <t>BANCO PACTUAL S A</t>
+        </is>
+      </c>
+      <c r="F23" s="49" t="inlineStr">
+        <is>
+          <t>FABIO MAGALHAES GOMES</t>
+        </is>
+      </c>
+      <c r="G23" s="89" t="inlineStr">
+        <is>
+          <t>1.991,48</t>
+        </is>
+      </c>
       <c r="H23" s="34" t="n"/>
       <c r="I23" s="32" t="n"/>
       <c r="J23" s="32" t="n"/>
@@ -3451,11 +3579,27 @@
       <c r="AC23" s="38" t="n"/>
       <c r="AD23" s="38" t="n"/>
       <c r="AE23" s="38" t="n"/>
-      <c r="AF23" s="90" t="n"/>
-      <c r="AG23" s="90" t="n"/>
-      <c r="AH23" s="32" t="n"/>
+      <c r="AF23" s="90" t="inlineStr">
+        <is>
+          <t>09970508116543</t>
+        </is>
+      </c>
+      <c r="AG23" s="90" t="inlineStr">
+        <is>
+          <t>00000000304</t>
+        </is>
+      </c>
+      <c r="AH23" s="32" t="inlineStr">
+        <is>
+          <t>23/05/2004</t>
+        </is>
+      </c>
       <c r="AI23" s="32" t="n"/>
-      <c r="AJ23" s="32" t="n"/>
+      <c r="AJ23" s="32" t="inlineStr">
+        <is>
+          <t>12447777053</t>
+        </is>
+      </c>
       <c r="AK23" s="32" t="n"/>
       <c r="AL23" s="32" t="n"/>
       <c r="AM23" s="32" t="n"/>
@@ -3493,13 +3637,33 @@
       <c r="BT23" s="1" t="n"/>
     </row>
     <row r="24" ht="15.95" customHeight="1" s="18">
-      <c r="A24" s="32" t="n"/>
+      <c r="A24" s="32" t="inlineStr">
+        <is>
+          <t>00018</t>
+        </is>
+      </c>
       <c r="B24" s="32" t="n"/>
       <c r="C24" s="32" t="n"/>
-      <c r="D24" s="32" t="n"/>
-      <c r="E24" s="49" t="n"/>
-      <c r="F24" s="49" t="n"/>
-      <c r="G24" s="89" t="n"/>
+      <c r="D24" s="32" t="inlineStr">
+        <is>
+          <t>000001747662011</t>
+        </is>
+      </c>
+      <c r="E24" s="49" t="inlineStr">
+        <is>
+          <t>BANCO PACTUAL S A</t>
+        </is>
+      </c>
+      <c r="F24" s="49" t="inlineStr">
+        <is>
+          <t>FERNANDO ANTONIO CLAUDIO JUNIOR</t>
+        </is>
+      </c>
+      <c r="G24" s="89" t="inlineStr">
+        <is>
+          <t>17.596,95</t>
+        </is>
+      </c>
       <c r="H24" s="34" t="n"/>
       <c r="I24" s="32" t="n"/>
       <c r="J24" s="32" t="n"/>
@@ -3524,11 +3688,27 @@
       <c r="AC24" s="38" t="n"/>
       <c r="AD24" s="38" t="n"/>
       <c r="AE24" s="38" t="n"/>
-      <c r="AF24" s="90" t="n"/>
-      <c r="AG24" s="90" t="n"/>
-      <c r="AH24" s="32" t="n"/>
+      <c r="AF24" s="90" t="inlineStr">
+        <is>
+          <t>09970508116543</t>
+        </is>
+      </c>
+      <c r="AG24" s="90" t="inlineStr">
+        <is>
+          <t>00000002609</t>
+        </is>
+      </c>
+      <c r="AH24" s="32" t="inlineStr">
+        <is>
+          <t>04/07/2012</t>
+        </is>
+      </c>
       <c r="AI24" s="32" t="n"/>
-      <c r="AJ24" s="32" t="n"/>
+      <c r="AJ24" s="32" t="inlineStr">
+        <is>
+          <t>00000000000</t>
+        </is>
+      </c>
       <c r="AK24" s="32" t="n"/>
       <c r="AL24" s="32" t="n"/>
       <c r="AM24" s="32" t="n"/>
@@ -3566,13 +3746,33 @@
       <c r="BT24" s="1" t="n"/>
     </row>
     <row r="25" ht="15.95" customHeight="1" s="18">
-      <c r="A25" s="32" t="n"/>
+      <c r="A25" s="32" t="inlineStr">
+        <is>
+          <t>00068</t>
+        </is>
+      </c>
       <c r="B25" s="32" t="n"/>
       <c r="C25" s="32" t="n"/>
-      <c r="D25" s="32" t="n"/>
-      <c r="E25" s="49" t="n"/>
-      <c r="F25" s="49" t="n"/>
-      <c r="G25" s="89" t="n"/>
+      <c r="D25" s="32" t="inlineStr">
+        <is>
+          <t>000001292412012</t>
+        </is>
+      </c>
+      <c r="E25" s="49" t="inlineStr">
+        <is>
+          <t>BANCO PACTUAL S A</t>
+        </is>
+      </c>
+      <c r="F25" s="49" t="inlineStr">
+        <is>
+          <t>JANE SANTOS SILVA</t>
+        </is>
+      </c>
+      <c r="G25" s="89" t="inlineStr">
+        <is>
+          <t>9.477,21</t>
+        </is>
+      </c>
       <c r="H25" s="34" t="n"/>
       <c r="I25" s="32" t="n"/>
       <c r="J25" s="32" t="n"/>
@@ -3597,11 +3797,27 @@
       <c r="AC25" s="38" t="n"/>
       <c r="AD25" s="38" t="n"/>
       <c r="AE25" s="38" t="n"/>
-      <c r="AF25" s="90" t="n"/>
-      <c r="AG25" s="90" t="n"/>
-      <c r="AH25" s="32" t="n"/>
+      <c r="AF25" s="90" t="inlineStr">
+        <is>
+          <t>09970508116543</t>
+        </is>
+      </c>
+      <c r="AG25" s="90" t="inlineStr">
+        <is>
+          <t>00000005454</t>
+        </is>
+      </c>
+      <c r="AH25" s="32" t="inlineStr">
+        <is>
+          <t>17/10/2013</t>
+        </is>
+      </c>
       <c r="AI25" s="32" t="n"/>
-      <c r="AJ25" s="32" t="n"/>
+      <c r="AJ25" s="32" t="inlineStr">
+        <is>
+          <t>00000000000</t>
+        </is>
+      </c>
       <c r="AK25" s="32" t="n"/>
       <c r="AL25" s="32" t="n"/>
       <c r="AM25" s="32" t="n"/>
@@ -3639,13 +3855,33 @@
       <c r="BT25" s="1" t="n"/>
     </row>
     <row r="26" ht="15.95" customHeight="1" s="18">
-      <c r="A26" s="32" t="n"/>
+      <c r="A26" s="32" t="inlineStr">
+        <is>
+          <t>00007</t>
+        </is>
+      </c>
       <c r="B26" s="32" t="n"/>
       <c r="C26" s="32" t="n"/>
-      <c r="D26" s="32" t="n"/>
-      <c r="E26" s="49" t="n"/>
-      <c r="F26" s="49" t="n"/>
-      <c r="G26" s="89" t="n"/>
+      <c r="D26" s="32" t="inlineStr">
+        <is>
+          <t>000000964962011</t>
+        </is>
+      </c>
+      <c r="E26" s="49" t="inlineStr">
+        <is>
+          <t>BANCO PACTUAL S A</t>
+        </is>
+      </c>
+      <c r="F26" s="49" t="inlineStr">
+        <is>
+          <t>JOSE A N SILVA FILHO</t>
+        </is>
+      </c>
+      <c r="G26" s="89" t="inlineStr">
+        <is>
+          <t>9.205,24</t>
+        </is>
+      </c>
       <c r="H26" s="34" t="n"/>
       <c r="I26" s="32" t="n"/>
       <c r="J26" s="32" t="n"/>
@@ -3670,11 +3906,27 @@
       <c r="AC26" s="38" t="n"/>
       <c r="AD26" s="38" t="n"/>
       <c r="AE26" s="38" t="n"/>
-      <c r="AF26" s="90" t="n"/>
-      <c r="AG26" s="90" t="n"/>
-      <c r="AH26" s="32" t="n"/>
+      <c r="AF26" s="90" t="inlineStr">
+        <is>
+          <t>09970508116543</t>
+        </is>
+      </c>
+      <c r="AG26" s="90" t="inlineStr">
+        <is>
+          <t>00000003087</t>
+        </is>
+      </c>
+      <c r="AH26" s="32" t="inlineStr">
+        <is>
+          <t>31/07/2012</t>
+        </is>
+      </c>
       <c r="AI26" s="32" t="n"/>
-      <c r="AJ26" s="32" t="n"/>
+      <c r="AJ26" s="32" t="inlineStr">
+        <is>
+          <t>13641828936</t>
+        </is>
+      </c>
       <c r="AK26" s="32" t="n"/>
       <c r="AL26" s="32" t="n"/>
       <c r="AM26" s="32" t="n"/>
@@ -3712,13 +3964,33 @@
       <c r="BT26" s="1" t="n"/>
     </row>
     <row r="27" ht="15.95" customHeight="1" s="18">
-      <c r="A27" s="32" t="n"/>
+      <c r="A27" s="32" t="inlineStr">
+        <is>
+          <t>00035</t>
+        </is>
+      </c>
       <c r="B27" s="32" t="n"/>
       <c r="C27" s="32" t="n"/>
-      <c r="D27" s="32" t="n"/>
-      <c r="E27" s="49" t="n"/>
-      <c r="F27" s="49" t="n"/>
-      <c r="G27" s="89" t="n"/>
+      <c r="D27" s="32" t="inlineStr">
+        <is>
+          <t>000000411662012</t>
+        </is>
+      </c>
+      <c r="E27" s="49" t="inlineStr">
+        <is>
+          <t>BANCO PACTUAL S A</t>
+        </is>
+      </c>
+      <c r="F27" s="49" t="inlineStr">
+        <is>
+          <t>LILIANE MATTOS RODRIGUES</t>
+        </is>
+      </c>
+      <c r="G27" s="89" t="inlineStr">
+        <is>
+          <t>9.460,52</t>
+        </is>
+      </c>
       <c r="H27" s="34" t="n"/>
       <c r="I27" s="32" t="n"/>
       <c r="J27" s="32" t="n"/>
@@ -3743,11 +4015,27 @@
       <c r="AC27" s="38" t="n"/>
       <c r="AD27" s="38" t="n"/>
       <c r="AE27" s="38" t="n"/>
-      <c r="AF27" s="90" t="n"/>
-      <c r="AG27" s="90" t="n"/>
-      <c r="AH27" s="32" t="n"/>
+      <c r="AF27" s="90" t="inlineStr">
+        <is>
+          <t>09970508116543</t>
+        </is>
+      </c>
+      <c r="AG27" s="90" t="inlineStr">
+        <is>
+          <t>00000006930</t>
+        </is>
+      </c>
+      <c r="AH27" s="32" t="inlineStr">
+        <is>
+          <t>25/05/2015</t>
+        </is>
+      </c>
       <c r="AI27" s="32" t="n"/>
-      <c r="AJ27" s="32" t="n"/>
+      <c r="AJ27" s="32" t="inlineStr">
+        <is>
+          <t>00000000000</t>
+        </is>
+      </c>
       <c r="AK27" s="32" t="n"/>
       <c r="AL27" s="32" t="n"/>
       <c r="AM27" s="32" t="n"/>
@@ -3785,13 +4073,33 @@
       <c r="BT27" s="1" t="n"/>
     </row>
     <row r="28" ht="15.75" customHeight="1" s="18">
-      <c r="A28" s="32" t="n"/>
+      <c r="A28" s="32" t="inlineStr">
+        <is>
+          <t>00018</t>
+        </is>
+      </c>
       <c r="B28" s="32" t="n"/>
       <c r="C28" s="32" t="n"/>
-      <c r="D28" s="32" t="n"/>
-      <c r="E28" s="49" t="n"/>
-      <c r="F28" s="49" t="n"/>
-      <c r="G28" s="89" t="n"/>
+      <c r="D28" s="32" t="inlineStr">
+        <is>
+          <t>000000112252008</t>
+        </is>
+      </c>
+      <c r="E28" s="49" t="inlineStr">
+        <is>
+          <t>BANCO PACTUAL S A</t>
+        </is>
+      </c>
+      <c r="F28" s="49" t="inlineStr">
+        <is>
+          <t>MARCELO CHAVES SOARES</t>
+        </is>
+      </c>
+      <c r="G28" s="89" t="inlineStr">
+        <is>
+          <t>8.593,39</t>
+        </is>
+      </c>
       <c r="H28" s="34" t="n"/>
       <c r="I28" s="32" t="n"/>
       <c r="J28" s="32" t="n"/>
@@ -3816,11 +4124,27 @@
       <c r="AC28" s="38" t="n"/>
       <c r="AD28" s="38" t="n"/>
       <c r="AE28" s="38" t="n"/>
-      <c r="AF28" s="90" t="n"/>
-      <c r="AG28" s="90" t="n"/>
-      <c r="AH28" s="32" t="n"/>
+      <c r="AF28" s="90" t="inlineStr">
+        <is>
+          <t>09970508116543</t>
+        </is>
+      </c>
+      <c r="AG28" s="90" t="inlineStr">
+        <is>
+          <t>00000001114</t>
+        </is>
+      </c>
+      <c r="AH28" s="32" t="inlineStr">
+        <is>
+          <t>25/05/2011</t>
+        </is>
+      </c>
       <c r="AI28" s="32" t="n"/>
-      <c r="AJ28" s="32" t="n"/>
+      <c r="AJ28" s="32" t="inlineStr">
+        <is>
+          <t>18194548549</t>
+        </is>
+      </c>
       <c r="AK28" s="32" t="n"/>
       <c r="AL28" s="32" t="n"/>
       <c r="AM28" s="32" t="n"/>
@@ -3858,13 +4182,33 @@
       <c r="BT28" s="1" t="n"/>
     </row>
     <row r="29" ht="15.75" customHeight="1" s="18">
-      <c r="A29" s="32" t="n"/>
+      <c r="A29" s="32" t="inlineStr">
+        <is>
+          <t>00066</t>
+        </is>
+      </c>
       <c r="B29" s="32" t="n"/>
       <c r="C29" s="32" t="n"/>
-      <c r="D29" s="32" t="n"/>
-      <c r="E29" s="49" t="n"/>
-      <c r="F29" s="49" t="n"/>
-      <c r="G29" s="89" t="n"/>
+      <c r="D29" s="32" t="inlineStr">
+        <is>
+          <t>000006040521999</t>
+        </is>
+      </c>
+      <c r="E29" s="49" t="inlineStr">
+        <is>
+          <t>BANCO PACTUAL S A</t>
+        </is>
+      </c>
+      <c r="F29" s="49" t="inlineStr">
+        <is>
+          <t>MARCELO F COLESI VASCONCELOS GALVAO</t>
+        </is>
+      </c>
+      <c r="G29" s="89" t="inlineStr">
+        <is>
+          <t>18.094,32</t>
+        </is>
+      </c>
       <c r="H29" s="34" t="n"/>
       <c r="I29" s="32" t="n"/>
       <c r="J29" s="32" t="n"/>
@@ -3889,11 +4233,27 @@
       <c r="AC29" s="38" t="n"/>
       <c r="AD29" s="38" t="n"/>
       <c r="AE29" s="38" t="n"/>
-      <c r="AF29" s="90" t="n"/>
-      <c r="AG29" s="90" t="n"/>
-      <c r="AH29" s="32" t="n"/>
+      <c r="AF29" s="90" t="inlineStr">
+        <is>
+          <t>09970508116543</t>
+        </is>
+      </c>
+      <c r="AG29" s="90" t="inlineStr">
+        <is>
+          <t>00000004300</t>
+        </is>
+      </c>
+      <c r="AH29" s="32" t="inlineStr">
+        <is>
+          <t>01/03/2013</t>
+        </is>
+      </c>
       <c r="AI29" s="32" t="n"/>
-      <c r="AJ29" s="32" t="n"/>
+      <c r="AJ29" s="32" t="inlineStr">
+        <is>
+          <t>00000000000</t>
+        </is>
+      </c>
       <c r="AK29" s="32" t="n"/>
       <c r="AL29" s="32" t="n"/>
       <c r="AM29" s="32" t="n"/>
@@ -3931,13 +4291,33 @@
       <c r="BT29" s="1" t="n"/>
     </row>
     <row r="30" ht="15.75" customHeight="1" s="18">
-      <c r="A30" s="32" t="n"/>
+      <c r="A30" s="32" t="inlineStr">
+        <is>
+          <t>00066</t>
+        </is>
+      </c>
       <c r="B30" s="32" t="n"/>
       <c r="C30" s="32" t="n"/>
-      <c r="D30" s="32" t="n"/>
-      <c r="E30" s="49" t="n"/>
-      <c r="F30" s="49" t="n"/>
-      <c r="G30" s="89" t="n"/>
+      <c r="D30" s="32" t="inlineStr">
+        <is>
+          <t>000000000601999</t>
+        </is>
+      </c>
+      <c r="E30" s="49" t="inlineStr">
+        <is>
+          <t>BANCO PACTUAL S A</t>
+        </is>
+      </c>
+      <c r="F30" s="49" t="inlineStr">
+        <is>
+          <t>MARCELO FRAZATTO COLESI V GALVAO</t>
+        </is>
+      </c>
+      <c r="G30" s="89" t="inlineStr">
+        <is>
+          <t>8.411,66</t>
+        </is>
+      </c>
       <c r="H30" s="34" t="n"/>
       <c r="I30" s="32" t="n"/>
       <c r="J30" s="32" t="n"/>
@@ -3962,11 +4342,27 @@
       <c r="AC30" s="38" t="n"/>
       <c r="AD30" s="38" t="n"/>
       <c r="AE30" s="38" t="n"/>
-      <c r="AF30" s="90" t="n"/>
-      <c r="AG30" s="90" t="n"/>
-      <c r="AH30" s="32" t="n"/>
+      <c r="AF30" s="90" t="inlineStr">
+        <is>
+          <t>09970508116543</t>
+        </is>
+      </c>
+      <c r="AG30" s="90" t="inlineStr">
+        <is>
+          <t>00000000495</t>
+        </is>
+      </c>
+      <c r="AH30" s="32" t="inlineStr">
+        <is>
+          <t>07/05/2006</t>
+        </is>
+      </c>
       <c r="AI30" s="32" t="n"/>
-      <c r="AJ30" s="32" t="n"/>
+      <c r="AJ30" s="32" t="inlineStr">
+        <is>
+          <t>12479624732</t>
+        </is>
+      </c>
       <c r="AK30" s="32" t="n"/>
       <c r="AL30" s="32" t="n"/>
       <c r="AM30" s="32" t="n"/>
@@ -4004,13 +4400,33 @@
       <c r="BT30" s="1" t="n"/>
     </row>
     <row r="31" ht="15.75" customHeight="1" s="18">
-      <c r="A31" s="32" t="n"/>
+      <c r="A31" s="32" t="inlineStr">
+        <is>
+          <t>00066</t>
+        </is>
+      </c>
       <c r="B31" s="32" t="n"/>
       <c r="C31" s="32" t="n"/>
-      <c r="D31" s="32" t="n"/>
-      <c r="E31" s="49" t="n"/>
-      <c r="F31" s="49" t="n"/>
-      <c r="G31" s="89" t="n"/>
+      <c r="D31" s="32" t="inlineStr">
+        <is>
+          <t>000000000601999</t>
+        </is>
+      </c>
+      <c r="E31" s="49" t="inlineStr">
+        <is>
+          <t>BANCO PACTUAL S A</t>
+        </is>
+      </c>
+      <c r="F31" s="49" t="inlineStr">
+        <is>
+          <t>MARCELO FRAZATTO COLESI V GALVAO</t>
+        </is>
+      </c>
+      <c r="G31" s="89" t="inlineStr">
+        <is>
+          <t>16.979,10</t>
+        </is>
+      </c>
       <c r="H31" s="34" t="n"/>
       <c r="I31" s="32" t="n"/>
       <c r="J31" s="32" t="n"/>
@@ -4035,11 +4451,27 @@
       <c r="AC31" s="38" t="n"/>
       <c r="AD31" s="38" t="n"/>
       <c r="AE31" s="38" t="n"/>
-      <c r="AF31" s="90" t="n"/>
-      <c r="AG31" s="90" t="n"/>
-      <c r="AH31" s="32" t="n"/>
+      <c r="AF31" s="90" t="inlineStr">
+        <is>
+          <t>09970508116543</t>
+        </is>
+      </c>
+      <c r="AG31" s="90" t="inlineStr">
+        <is>
+          <t>00000000908</t>
+        </is>
+      </c>
+      <c r="AH31" s="32" t="inlineStr">
+        <is>
+          <t>11/02/2009</t>
+        </is>
+      </c>
       <c r="AI31" s="32" t="n"/>
-      <c r="AJ31" s="32" t="n"/>
+      <c r="AJ31" s="32" t="inlineStr">
+        <is>
+          <t>12479624732</t>
+        </is>
+      </c>
       <c r="AK31" s="32" t="n"/>
       <c r="AL31" s="32" t="n"/>
       <c r="AM31" s="32" t="n"/>
@@ -4077,13 +4509,33 @@
       <c r="BT31" s="1" t="n"/>
     </row>
     <row r="32" ht="15.75" customHeight="1" s="18">
-      <c r="A32" s="32" t="n"/>
+      <c r="A32" s="32" t="inlineStr">
+        <is>
+          <t>00066</t>
+        </is>
+      </c>
       <c r="B32" s="32" t="n"/>
       <c r="C32" s="32" t="n"/>
-      <c r="D32" s="32" t="n"/>
-      <c r="E32" s="49" t="n"/>
-      <c r="F32" s="49" t="n"/>
-      <c r="G32" s="89" t="n"/>
+      <c r="D32" s="32" t="inlineStr">
+        <is>
+          <t>000006041371999</t>
+        </is>
+      </c>
+      <c r="E32" s="49" t="inlineStr">
+        <is>
+          <t>BANCO PACTUAL S A</t>
+        </is>
+      </c>
+      <c r="F32" s="49" t="inlineStr">
+        <is>
+          <t>MARCELO FRAZATTO COLEZI VASCONCELOS G</t>
+        </is>
+      </c>
+      <c r="G32" s="89" t="inlineStr">
+        <is>
+          <t>18.411,14</t>
+        </is>
+      </c>
       <c r="H32" s="34" t="n"/>
       <c r="I32" s="32" t="n"/>
       <c r="J32" s="32" t="n"/>
@@ -4108,11 +4560,27 @@
       <c r="AC32" s="38" t="n"/>
       <c r="AD32" s="38" t="n"/>
       <c r="AE32" s="38" t="n"/>
-      <c r="AF32" s="90" t="n"/>
-      <c r="AG32" s="90" t="n"/>
-      <c r="AH32" s="32" t="n"/>
+      <c r="AF32" s="90" t="inlineStr">
+        <is>
+          <t>09970508116543</t>
+        </is>
+      </c>
+      <c r="AG32" s="90" t="inlineStr">
+        <is>
+          <t>00000003168</t>
+        </is>
+      </c>
+      <c r="AH32" s="32" t="inlineStr">
+        <is>
+          <t>07/08/2012</t>
+        </is>
+      </c>
       <c r="AI32" s="32" t="n"/>
-      <c r="AJ32" s="32" t="n"/>
+      <c r="AJ32" s="32" t="inlineStr">
+        <is>
+          <t>00000000000</t>
+        </is>
+      </c>
       <c r="AK32" s="32" t="n"/>
       <c r="AL32" s="32" t="n"/>
       <c r="AM32" s="32" t="n"/>
@@ -4150,13 +4618,33 @@
       <c r="BT32" s="1" t="n"/>
     </row>
     <row r="33" ht="15.75" customHeight="1" s="18">
-      <c r="A33" s="32" t="n"/>
+      <c r="A33" s="32" t="inlineStr">
+        <is>
+          <t>00066</t>
+        </is>
+      </c>
       <c r="B33" s="32" t="n"/>
       <c r="C33" s="32" t="n"/>
-      <c r="D33" s="32" t="n"/>
-      <c r="E33" s="49" t="n"/>
-      <c r="F33" s="49" t="n"/>
-      <c r="G33" s="89" t="n"/>
+      <c r="D33" s="32" t="inlineStr">
+        <is>
+          <t>000006041371999</t>
+        </is>
+      </c>
+      <c r="E33" s="49" t="inlineStr">
+        <is>
+          <t>BANCO PACTUAL S A</t>
+        </is>
+      </c>
+      <c r="F33" s="49" t="inlineStr">
+        <is>
+          <t>MARCELO FRAZATTO COLEZI VASCONCELOS G</t>
+        </is>
+      </c>
+      <c r="G33" s="89" t="inlineStr">
+        <is>
+          <t>18.411,14</t>
+        </is>
+      </c>
       <c r="H33" s="34" t="n"/>
       <c r="I33" s="32" t="n"/>
       <c r="J33" s="32" t="n"/>
@@ -4181,11 +4669,27 @@
       <c r="AC33" s="38" t="n"/>
       <c r="AD33" s="38" t="n"/>
       <c r="AE33" s="38" t="n"/>
-      <c r="AF33" s="90" t="n"/>
-      <c r="AG33" s="90" t="n"/>
-      <c r="AH33" s="32" t="n"/>
+      <c r="AF33" s="90" t="inlineStr">
+        <is>
+          <t>09970508116543</t>
+        </is>
+      </c>
+      <c r="AG33" s="90" t="inlineStr">
+        <is>
+          <t>00000003249</t>
+        </is>
+      </c>
+      <c r="AH33" s="32" t="inlineStr">
+        <is>
+          <t>07/08/2012</t>
+        </is>
+      </c>
       <c r="AI33" s="32" t="n"/>
-      <c r="AJ33" s="32" t="n"/>
+      <c r="AJ33" s="32" t="inlineStr">
+        <is>
+          <t>00000000000</t>
+        </is>
+      </c>
       <c r="AK33" s="32" t="n"/>
       <c r="AL33" s="32" t="n"/>
       <c r="AM33" s="32" t="n"/>
@@ -4223,13 +4727,33 @@
       <c r="BT33" s="1" t="n"/>
     </row>
     <row r="34" ht="15.75" customHeight="1" s="18">
-      <c r="A34" s="32" t="n"/>
+      <c r="A34" s="32" t="inlineStr">
+        <is>
+          <t>00062</t>
+        </is>
+      </c>
       <c r="B34" s="32" t="n"/>
       <c r="C34" s="32" t="n"/>
-      <c r="D34" s="32" t="n"/>
-      <c r="E34" s="49" t="n"/>
-      <c r="F34" s="49" t="n"/>
-      <c r="G34" s="89" t="n"/>
+      <c r="D34" s="32" t="inlineStr">
+        <is>
+          <t>000000006172012</t>
+        </is>
+      </c>
+      <c r="E34" s="49" t="inlineStr">
+        <is>
+          <t>BANCO PACTUAL S A</t>
+        </is>
+      </c>
+      <c r="F34" s="49" t="inlineStr">
+        <is>
+          <t>MARIANA FERREIRA CRUZ LIMA</t>
+        </is>
+      </c>
+      <c r="G34" s="89" t="inlineStr">
+        <is>
+          <t>9.113,91</t>
+        </is>
+      </c>
       <c r="H34" s="34" t="n"/>
       <c r="I34" s="32" t="n"/>
       <c r="J34" s="32" t="n"/>
@@ -4254,11 +4778,27 @@
       <c r="AC34" s="38" t="n"/>
       <c r="AD34" s="38" t="n"/>
       <c r="AE34" s="38" t="n"/>
-      <c r="AF34" s="90" t="n"/>
-      <c r="AG34" s="90" t="n"/>
-      <c r="AH34" s="32" t="n"/>
+      <c r="AF34" s="90" t="inlineStr">
+        <is>
+          <t>09970508116543</t>
+        </is>
+      </c>
+      <c r="AG34" s="90" t="inlineStr">
+        <is>
+          <t>00000003915</t>
+        </is>
+      </c>
+      <c r="AH34" s="32" t="inlineStr">
+        <is>
+          <t>04/12/2012</t>
+        </is>
+      </c>
       <c r="AI34" s="32" t="n"/>
-      <c r="AJ34" s="32" t="n"/>
+      <c r="AJ34" s="32" t="inlineStr">
+        <is>
+          <t>00000000000</t>
+        </is>
+      </c>
       <c r="AK34" s="32" t="n"/>
       <c r="AL34" s="32" t="n"/>
       <c r="AM34" s="32" t="n"/>
@@ -4296,13 +4836,33 @@
       <c r="BT34" s="1" t="n"/>
     </row>
     <row r="35" ht="15.75" customHeight="1" s="18">
-      <c r="A35" s="32" t="n"/>
+      <c r="A35" s="32" t="inlineStr">
+        <is>
+          <t>00021</t>
+        </is>
+      </c>
       <c r="B35" s="32" t="n"/>
       <c r="C35" s="32" t="n"/>
-      <c r="D35" s="32" t="n"/>
-      <c r="E35" s="49" t="n"/>
-      <c r="F35" s="49" t="n"/>
-      <c r="G35" s="89" t="n"/>
+      <c r="D35" s="32" t="inlineStr">
+        <is>
+          <t>000010688182014</t>
+        </is>
+      </c>
+      <c r="E35" s="49" t="inlineStr">
+        <is>
+          <t>BANCO PACTUAL S A</t>
+        </is>
+      </c>
+      <c r="F35" s="49" t="inlineStr">
+        <is>
+          <t>RODRIGO GUSTAVO SANTOS SARRAT</t>
+        </is>
+      </c>
+      <c r="G35" s="89" t="inlineStr">
+        <is>
+          <t>18.751,25</t>
+        </is>
+      </c>
       <c r="H35" s="34" t="n"/>
       <c r="I35" s="32" t="n"/>
       <c r="J35" s="32" t="n"/>
@@ -4327,11 +4887,27 @@
       <c r="AC35" s="38" t="n"/>
       <c r="AD35" s="38" t="n"/>
       <c r="AE35" s="38" t="n"/>
-      <c r="AF35" s="90" t="n"/>
-      <c r="AG35" s="90" t="n"/>
-      <c r="AH35" s="32" t="n"/>
+      <c r="AF35" s="90" t="inlineStr">
+        <is>
+          <t>09970508116543</t>
+        </is>
+      </c>
+      <c r="AG35" s="90" t="inlineStr">
+        <is>
+          <t>00000008208</t>
+        </is>
+      </c>
+      <c r="AH35" s="32" t="inlineStr">
+        <is>
+          <t>29/07/2015</t>
+        </is>
+      </c>
       <c r="AI35" s="32" t="n"/>
-      <c r="AJ35" s="32" t="n"/>
+      <c r="AJ35" s="32" t="inlineStr">
+        <is>
+          <t>00000000000</t>
+        </is>
+      </c>
       <c r="AK35" s="32" t="n"/>
       <c r="AL35" s="32" t="n"/>
       <c r="AM35" s="32" t="n"/>
@@ -4369,13 +4945,33 @@
       <c r="BT35" s="1" t="n"/>
     </row>
     <row r="36" ht="15.75" customHeight="1" s="18">
-      <c r="A36" s="32" t="n"/>
+      <c r="A36" s="32" t="inlineStr">
+        <is>
+          <t>00072</t>
+        </is>
+      </c>
       <c r="B36" s="32" t="n"/>
       <c r="C36" s="32" t="n"/>
-      <c r="D36" s="32" t="n"/>
-      <c r="E36" s="49" t="n"/>
-      <c r="F36" s="49" t="n"/>
-      <c r="G36" s="89" t="n"/>
+      <c r="D36" s="32" t="inlineStr">
+        <is>
+          <t>000001144862010</t>
+        </is>
+      </c>
+      <c r="E36" s="49" t="inlineStr">
+        <is>
+          <t>BANCO PACTUAL S A</t>
+        </is>
+      </c>
+      <c r="F36" s="49" t="inlineStr">
+        <is>
+          <t>SONIA MOREIRA SANTANA ALMEIDA</t>
+        </is>
+      </c>
+      <c r="G36" s="89" t="inlineStr">
+        <is>
+          <t>13.745,27</t>
+        </is>
+      </c>
       <c r="H36" s="34" t="n"/>
       <c r="I36" s="32" t="n"/>
       <c r="J36" s="32" t="n"/>
@@ -4400,11 +4996,27 @@
       <c r="AC36" s="38" t="n"/>
       <c r="AD36" s="38" t="n"/>
       <c r="AE36" s="38" t="n"/>
-      <c r="AF36" s="90" t="n"/>
-      <c r="AG36" s="90" t="n"/>
-      <c r="AH36" s="32" t="n"/>
+      <c r="AF36" s="90" t="inlineStr">
+        <is>
+          <t>09970508116543</t>
+        </is>
+      </c>
+      <c r="AG36" s="90" t="inlineStr">
+        <is>
+          <t>00000004210</t>
+        </is>
+      </c>
+      <c r="AH36" s="32" t="inlineStr">
+        <is>
+          <t>05/02/2013</t>
+        </is>
+      </c>
       <c r="AI36" s="32" t="n"/>
-      <c r="AJ36" s="32" t="n"/>
+      <c r="AJ36" s="32" t="inlineStr">
+        <is>
+          <t>00000000000</t>
+        </is>
+      </c>
       <c r="AK36" s="32" t="n"/>
       <c r="AL36" s="32" t="n"/>
       <c r="AM36" s="32" t="n"/>
@@ -4442,13 +5054,33 @@
       <c r="BT36" s="1" t="n"/>
     </row>
     <row r="37" ht="15.75" customHeight="1" s="18">
-      <c r="A37" s="32" t="n"/>
+      <c r="A37" s="32" t="inlineStr">
+        <is>
+          <t>00069</t>
+        </is>
+      </c>
       <c r="B37" s="32" t="n"/>
       <c r="C37" s="32" t="n"/>
-      <c r="D37" s="32" t="n"/>
-      <c r="E37" s="49" t="n"/>
-      <c r="F37" s="49" t="n"/>
-      <c r="G37" s="89" t="n"/>
+      <c r="D37" s="32" t="inlineStr">
+        <is>
+          <t>000037300892009</t>
+        </is>
+      </c>
+      <c r="E37" s="49" t="inlineStr">
+        <is>
+          <t>BANCO PACTUAL S A</t>
+        </is>
+      </c>
+      <c r="F37" s="49" t="inlineStr">
+        <is>
+          <t>TATIANE APARECIDA DIAN HERMANE</t>
+        </is>
+      </c>
+      <c r="G37" s="89" t="inlineStr">
+        <is>
+          <t>9.046,83</t>
+        </is>
+      </c>
       <c r="H37" s="34" t="n"/>
       <c r="I37" s="32" t="n"/>
       <c r="J37" s="32" t="n"/>
@@ -4473,11 +5105,27 @@
       <c r="AC37" s="38" t="n"/>
       <c r="AD37" s="38" t="n"/>
       <c r="AE37" s="38" t="n"/>
-      <c r="AF37" s="90" t="n"/>
-      <c r="AG37" s="90" t="n"/>
-      <c r="AH37" s="32" t="n"/>
+      <c r="AF37" s="90" t="inlineStr">
+        <is>
+          <t>09970508116543</t>
+        </is>
+      </c>
+      <c r="AG37" s="90" t="inlineStr">
+        <is>
+          <t>00000004482</t>
+        </is>
+      </c>
+      <c r="AH37" s="32" t="inlineStr">
+        <is>
+          <t>01/03/2013</t>
+        </is>
+      </c>
       <c r="AI37" s="32" t="n"/>
-      <c r="AJ37" s="32" t="n"/>
+      <c r="AJ37" s="32" t="inlineStr">
+        <is>
+          <t>00000000000</t>
+        </is>
+      </c>
       <c r="AK37" s="32" t="n"/>
       <c r="AL37" s="32" t="n"/>
       <c r="AM37" s="32" t="n"/>

</xml_diff>